<commit_message>
Last 3 years changes + mvn -> gradle some things might not work though :( need more tests
</commit_message>
<xml_diff>
--- a/ee.fj.io/ee.fj.io.tablereader/src/test/resources/simple.xlsx
+++ b/ee.fj.io/ee.fj.io.tablereader/src/test/resources/simple.xlsx
@@ -17,7 +17,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Šašikul on kole nälg</t>
+    <r>
+      <t>Šašlikul on kole nälg </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="2"/>
+      </rPr>
+      <t>õäöüÕÄÖÜ</t>
+    </r>
   </si>
   <si>
     <t>Tüina</t>
@@ -35,7 +46,7 @@
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YYYY\ HH:MM:SS"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -60,6 +71,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -148,12 +165,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0510204081633"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>